<commit_message>
se arreglo error de scripts.
</commit_message>
<xml_diff>
--- a/excel/GUI Automated Testing -Project creation.xlsx
+++ b/excel/GUI Automated Testing -Project creation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUI_PC_AN_001" sheetId="1" r:id="rId1"/>
@@ -924,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -5631,7 +5631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>